<commit_message>
1. Use of Global Object 2. Password encryption 3. Update Range maps (removed optional params)
</commit_message>
<xml_diff>
--- a/TC_CreateNewLead/Main.rvl.xlsx
+++ b/TC_CreateNewLead/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="104">
   <si>
     <t>Flow</t>
   </si>
@@ -310,6 +310,21 @@
   </si>
   <si>
     <t>Refresh</t>
+  </si>
+  <si>
+    <t>Crm</t>
+  </si>
+  <si>
+    <t>OpenEntity</t>
+  </si>
+  <si>
+    <t>LaunchSales</t>
+  </si>
+  <si>
+    <t>ChangeArea</t>
+  </si>
+  <si>
+    <t>ClickButton</t>
   </si>
 </sst>
 </file>
@@ -330,7 +345,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="233">
+  <borders count="252">
     <border>
       <left/>
       <right/>
@@ -570,11 +585,30 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="233">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -808,6 +842,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="230" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="231" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="232" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="234" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="235" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="236" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="238" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="239" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="240" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="241" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="242" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="243" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="244" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="246" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="247" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="248" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="250" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="251" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,7 +870,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H49"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.453125" customWidth="true"/>
@@ -1023,267 +1076,300 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="224"/>
+      <c r="A14" s="221" t="s">
+        <v>72</v>
+      </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="222"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="33"/>
+      <c r="B18" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="40"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="48"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="57"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="64"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="229"/>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="230"/>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
         <v>82</v>
       </c>
-      <c r="G14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="225"/>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="226"/>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" t="s">
-        <v>82</v>
-      </c>
-      <c r="G16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="227"/>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="221" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="222"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="24"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="25"/>
-      <c r="B21" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="32"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="33"/>
-      <c r="B22" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="40"/>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="41"/>
-      <c r="B23" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="48"/>
+      <c r="A23" s="231"/>
     </row>
     <row r="24">
-      <c r="A24" s="57"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="64"/>
+      <c r="A24" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="72"/>
     </row>
     <row r="25">
-      <c r="A25" s="229"/>
+      <c r="A25" s="161" t="s">
+        <v>7</v>
+      </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="230"/>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" t="s">
-        <v>82</v>
-      </c>
-      <c r="G26" t="s">
-        <v>95</v>
-      </c>
+      <c r="A26" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="79" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="80"/>
     </row>
     <row r="27">
-      <c r="A27" s="231"/>
+      <c r="A27" s="162" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="67" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="68" t="s">
+      <c r="A28" s="163" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="72"/>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="161" t="s">
+      <c r="A29" s="164" t="s">
         <v>7</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
         <v>23</v>
@@ -1295,42 +1381,41 @@
         <v>75</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="73" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="76" t="s">
+      <c r="A30" s="165" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="77" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="79" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="80"/>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="162" t="s">
+      <c r="A31" s="166" t="s">
         <v>7</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
         <v>23</v>
@@ -1342,44 +1427,45 @@
         <v>75</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="163" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="A32" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="83" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" t="s">
-        <v>7</v>
-      </c>
+      <c r="E32" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="87" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="88"/>
     </row>
     <row r="33">
-      <c r="A33" s="164" t="s">
+      <c r="A33" s="168" t="s">
         <v>7</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
         <v>24</v>
@@ -1388,427 +1474,334 @@
         <v>75</v>
       </c>
       <c r="G33" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="165" t="s">
+      <c r="A34" s="171" t="s">
         <v>7</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" t="s">
+        <v>75</v>
+      </c>
+      <c r="G34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="189" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" t="s">
         <v>22</v>
       </c>
-      <c r="E34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="166" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" t="s">
-        <v>23</v>
-      </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="190" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="89"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="91"/>
+      <c r="D38" s="92"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="95"/>
+      <c r="H38" s="96"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="97"/>
+      <c r="B39" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="99" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="100" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="102" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="103" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="104"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="106" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="107" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="108" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="109" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="110" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="111" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="112"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="232"/>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" t="s">
+        <v>94</v>
+      </c>
+      <c r="F41" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="113" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="114" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="115" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="116" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="117" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="G35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="84" t="s">
+      <c r="G42" s="119" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="120"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="194" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>51</v>
+      </c>
+      <c r="F43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="195" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="85" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="87" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="88"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="168" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" t="s">
-        <v>75</v>
-      </c>
-      <c r="G37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="171" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="189" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="196" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" t="s">
         <v>22</v>
       </c>
-      <c r="E39" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="190" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="175" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="89"/>
-      <c r="B42" s="90"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="92"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="94"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="96"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="97"/>
-      <c r="B43" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="99" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="100" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="101" t="s">
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="121"/>
+      <c r="B46" s="122"/>
+      <c r="C46" s="123"/>
+      <c r="D46" s="124"/>
+      <c r="E46" s="125"/>
+      <c r="F46" s="126"/>
+      <c r="G46" s="127"/>
+      <c r="H46" s="128"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="129"/>
+      <c r="B47" s="130" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="131" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="132" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="F43" s="102" t="s">
+      <c r="F47" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="103" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="104"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="105" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="106" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="D44" s="108" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="109" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="110" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="112"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="232"/>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>89</v>
-      </c>
-      <c r="D45" t="s">
-        <v>93</v>
-      </c>
-      <c r="E45" t="s">
-        <v>94</v>
-      </c>
-      <c r="F45" t="s">
-        <v>82</v>
-      </c>
-      <c r="G45" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="113" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="114" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="115" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46" s="116" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" s="117" t="s">
-        <v>49</v>
-      </c>
-      <c r="F46" s="118" t="s">
-        <v>75</v>
-      </c>
-      <c r="G46" s="119" t="s">
-        <v>21</v>
-      </c>
-      <c r="H46" s="120"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="194" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" t="s">
-        <v>51</v>
-      </c>
-      <c r="F47" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" t="s">
-        <v>21</v>
-      </c>
+      <c r="G47" s="135" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="136"/>
     </row>
     <row r="48">
-      <c r="A48" s="195" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" t="s">
-        <v>7</v>
-      </c>
+      <c r="A48" s="137"/>
+      <c r="B48" s="138" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="139" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="140" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" s="141" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="142" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="143" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="144"/>
     </row>
     <row r="49">
-      <c r="A49" s="196" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>53</v>
-      </c>
-      <c r="D49" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="121"/>
-      <c r="B50" s="122"/>
-      <c r="C50" s="123"/>
-      <c r="D50" s="124"/>
-      <c r="E50" s="125"/>
-      <c r="F50" s="126"/>
-      <c r="G50" s="127"/>
-      <c r="H50" s="128"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="129"/>
-      <c r="B51" s="130" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="131" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="132" t="s">
-        <v>16</v>
-      </c>
-      <c r="E51" s="133" t="s">
-        <v>17</v>
-      </c>
-      <c r="F51" s="134" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="135" t="s">
-        <v>55</v>
-      </c>
-      <c r="H51" s="136"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="137"/>
-      <c r="B52" s="138" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="139" t="s">
-        <v>42</v>
-      </c>
-      <c r="D52" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="E52" s="141" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" s="142" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52" s="143" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="144"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="153"/>
-      <c r="B53" s="154"/>
-      <c r="C53" s="155"/>
-      <c r="D53" s="156"/>
-      <c r="E53" s="157"/>
-      <c r="F53" s="158"/>
-      <c r="G53" s="159"/>
-      <c r="H53" s="160"/>
+      <c r="A49" s="153"/>
+      <c r="B49" s="154"/>
+      <c r="C49" s="155"/>
+      <c r="D49" s="156"/>
+      <c r="E49" s="157"/>
+      <c r="F49" s="158"/>
+      <c r="G49" s="159"/>
+      <c r="H49" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
Synchronized with demo rep
</commit_message>
<xml_diff>
--- a/TC_CreateNewLead/Main.rvl.xlsx
+++ b/TC_CreateNewLead/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="111">
   <si>
     <t>Flow</t>
   </si>
@@ -325,6 +325,27 @@
   </si>
   <si>
     <t>ClickButton</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>15000</t>
+  </si>
+  <si>
+    <t>timeout</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>sleepTimeIfFound</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>20000</t>
   </si>
 </sst>
 </file>
@@ -345,7 +366,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="252">
+  <borders count="262">
     <border>
       <left/>
       <right/>
@@ -604,11 +625,21 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -861,6 +892,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="250" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="251" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="252" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="254" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="255" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="256" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="258" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="259" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="260" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="261" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,7 +911,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H53"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.453125" customWidth="true"/>
@@ -1124,104 +1165,104 @@
       <c r="H16" s="24"/>
     </row>
     <row r="17">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="27" t="s">
+      <c r="A17" s="253"/>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D18" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E18" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F18" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G18" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="32"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="35" t="s">
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="33"/>
+      <c r="B19" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D19" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E19" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F19" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G19" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="40"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="43" t="s">
+      <c r="H19" s="40"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="41"/>
+      <c r="B20" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D20" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="45" t="s">
+      <c r="E20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F20" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="47" t="s">
+      <c r="G20" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="48"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="57"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="64"/>
+      <c r="H20" s="48"/>
     </row>
     <row r="21">
-      <c r="A21" s="229"/>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" t="s">
-        <v>39</v>
-      </c>
+      <c r="A21" s="57"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="64"/>
     </row>
     <row r="22">
-      <c r="A22" s="230"/>
+      <c r="A22" s="229"/>
       <c r="B22" t="s">
         <v>3</v>
       </c>
@@ -1229,101 +1270,84 @@
         <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="256"/>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" t="s">
         <v>82</v>
       </c>
-      <c r="G22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="231"/>
+      <c r="G23" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="67" t="s">
+      <c r="A24" s="257"/>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="231"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="68" t="s">
+      <c r="D26" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="72"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="161" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="E26" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="72"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="161" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
         <v>21</v>
-      </c>
-      <c r="D25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="73" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="77" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="79" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="80"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="162" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
       </c>
       <c r="D27" t="s">
         <v>23</v>
@@ -1335,41 +1359,42 @@
         <v>75</v>
       </c>
       <c r="G27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="75" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="163" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="D28" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
+      <c r="E28" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="79" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="80"/>
     </row>
     <row r="29">
-      <c r="A29" s="164" t="s">
+      <c r="A29" s="162" t="s">
         <v>7</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
         <v>23</v>
@@ -1381,18 +1406,18 @@
         <v>75</v>
       </c>
       <c r="G29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="163" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="165" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>30</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
@@ -1408,14 +1433,14 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="164" t="s">
         <v>7</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
         <v>23</v>
@@ -1427,45 +1452,44 @@
         <v>75</v>
       </c>
       <c r="G31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="165" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="84" t="s">
+      <c r="D32" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="85" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="87" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="88"/>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="168" t="s">
+      <c r="A33" s="166" t="s">
         <v>7</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
         <v>24</v>
@@ -1474,87 +1498,88 @@
         <v>75</v>
       </c>
       <c r="G33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="83" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="87" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="88"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="168" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="171" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="171" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
         <v>41</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>34</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E36" t="s">
         <v>24</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F36" t="s">
         <v>75</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="189" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="37">
+      <c r="A37" s="189" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
         <v>45</v>
-      </c>
-      <c r="D35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="190" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="175" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>39</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -1570,161 +1595,168 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="89"/>
-      <c r="B38" s="90"/>
-      <c r="C38" s="91"/>
-      <c r="D38" s="92"/>
-      <c r="E38" s="93"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="96"/>
+      <c r="A38" s="190" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="97"/>
-      <c r="B39" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="99" t="s">
+      <c r="A39" s="175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="89"/>
+      <c r="B40" s="90" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="91" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="92" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="93" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="94" t="s">
+        <v>82</v>
+      </c>
+      <c r="G40" s="95" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" s="96"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="97"/>
+      <c r="B41" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="100" t="s">
+      <c r="D41" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="101" t="s">
+      <c r="E41" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="102" t="s">
+      <c r="F41" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="103" t="s">
+      <c r="G41" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="H39" s="104"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="105" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="106" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="107" t="s">
+      <c r="H41" s="104"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="258"/>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" t="s">
+        <v>94</v>
+      </c>
+      <c r="F42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="106" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="107" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="108" t="s">
+      <c r="D43" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="E40" s="109" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="110" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="112"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="232"/>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="E43" s="109" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="110" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="111" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="112"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="259"/>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
         <v>89</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D44" t="s">
         <v>93</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E44" t="s">
         <v>94</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F44" t="s">
         <v>82</v>
       </c>
-      <c r="G41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="113" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="114" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="115" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="116" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="117" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="118" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="119" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" s="120"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="194" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" t="s">
-        <v>51</v>
-      </c>
-      <c r="F43" t="s">
-        <v>12</v>
-      </c>
-      <c r="G43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="195" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" t="s">
-        <v>7</v>
-      </c>
       <c r="G44" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="196" t="s">
-        <v>7</v>
-      </c>
+      <c r="A45" s="260"/>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -1740,68 +1772,160 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="121"/>
-      <c r="B46" s="122"/>
-      <c r="C46" s="123"/>
-      <c r="D46" s="124"/>
-      <c r="E46" s="125"/>
-      <c r="F46" s="126"/>
-      <c r="G46" s="127"/>
-      <c r="H46" s="128"/>
+      <c r="A46" s="232"/>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" t="s">
+        <v>94</v>
+      </c>
+      <c r="F46" t="s">
+        <v>82</v>
+      </c>
+      <c r="G46" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="129"/>
-      <c r="B47" s="130" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="131" t="s">
+      <c r="A47" s="113" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="114" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="115" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="116" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" s="117" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="118" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" s="119" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47" s="120"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="194" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" t="s">
+        <v>51</v>
+      </c>
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="195" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="196" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="121"/>
+      <c r="B51" s="122"/>
+      <c r="C51" s="123"/>
+      <c r="D51" s="124"/>
+      <c r="E51" s="125"/>
+      <c r="F51" s="126"/>
+      <c r="G51" s="127"/>
+      <c r="H51" s="128"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="129"/>
+      <c r="B52" s="130" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="131" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="132" t="s">
+      <c r="D52" s="132" t="s">
         <v>100</v>
       </c>
-      <c r="E47" s="133" t="s">
+      <c r="E52" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="F47" s="134" t="s">
+      <c r="F52" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="G47" s="135" t="s">
+      <c r="G52" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="H47" s="136"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="137"/>
-      <c r="B48" s="138" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="139" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="E48" s="141" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="142" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="143" t="s">
-        <v>7</v>
-      </c>
-      <c r="H48" s="144"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="153"/>
-      <c r="B49" s="154"/>
-      <c r="C49" s="155"/>
-      <c r="D49" s="156"/>
-      <c r="E49" s="157"/>
-      <c r="F49" s="158"/>
-      <c r="G49" s="159"/>
-      <c r="H49" s="160"/>
+      <c r="H52" s="136"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="153"/>
+      <c r="B53" s="154"/>
+      <c r="C53" s="155"/>
+      <c r="D53" s="156"/>
+      <c r="E53" s="157"/>
+      <c r="F53" s="158"/>
+      <c r="G53" s="159"/>
+      <c r="H53" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>